<commit_message>
Updated scrapper API key & update Auto_scrap_HomeDepot.py
</commit_message>
<xml_diff>
--- a/XX_Master_database/Wholesaler_Database.xlsx
+++ b/XX_Master_database/Wholesaler_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/00_Scrapping_git/XX_Master_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1407" documentId="8_{B63EC7D8-7803-4775-989F-2C2416119993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF12493E-5CC5-4207-ADD9-ED89501033C2}"/>
+  <xr:revisionPtr revIDLastSave="1419" documentId="8_{B63EC7D8-7803-4775-989F-2C2416119993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BCDF189-B6DA-450A-8990-3E54315EC67C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="1" xr2:uid="{BB750D66-C71B-4412-8809-92E47E37BD8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB750D66-C71B-4412-8809-92E47E37BD8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitors" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Competitors!$A$1:$Q$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Competitors!$A$1:$R$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="271">
   <si>
     <t>GMX20902</t>
   </si>
@@ -846,6 +846,15 @@
   </si>
   <si>
     <t>135010007, 103580000</t>
+  </si>
+  <si>
+    <t>URL_img</t>
+  </si>
+  <si>
+    <t>URL_Img</t>
+  </si>
+  <si>
+    <t>https://www.mansfieldplumbing.com/wp-content/uploads/2020/04/Alto_Combo_130-3173_001_Web-1.jpg</t>
   </si>
 </sst>
 </file>
@@ -5076,11 +5085,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB033180-4452-49A4-8BEB-F48FDF308044}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5099,12 +5108,13 @@
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="60.140625" customWidth="1"/>
     <col min="14" max="14" width="169" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="82.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -5146,16 +5156,19 @@
         <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -5201,15 +5214,16 @@
       <c r="N2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P2" s="28">
+      <c r="Q2" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q2" s="15"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="15"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -5255,15 +5269,16 @@
       <c r="N3" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="17"/>
+      <c r="P3" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P3" s="28">
+      <c r="Q3" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q3" s="15"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -5309,15 +5324,16 @@
       <c r="N4" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="17"/>
+      <c r="P4" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P4" s="28">
+      <c r="Q4" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q4" s="15"/>
-    </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R4" s="15"/>
+    </row>
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
@@ -5362,15 +5378,16 @@
       <c r="N5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="17"/>
+      <c r="P5" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P5" s="28">
+      <c r="Q5" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q5" s="15"/>
-    </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
@@ -5416,15 +5433,16 @@
       <c r="N6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="17"/>
+      <c r="P6" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P6" s="28">
+      <c r="Q6" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
@@ -5470,15 +5488,16 @@
       <c r="N7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="15"/>
+      <c r="P7" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P7" s="28">
+      <c r="Q7" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q7" s="15"/>
-    </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="15"/>
+    </row>
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -5524,15 +5543,16 @@
       <c r="N8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="15"/>
+      <c r="P8" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P8" s="28">
+      <c r="Q8" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q8" s="15"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
@@ -5578,15 +5598,16 @@
       <c r="N9" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="17"/>
+      <c r="P9" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P9" s="28">
+      <c r="Q9" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>4</v>
       </c>
@@ -5626,17 +5647,18 @@
         <v>221</v>
       </c>
       <c r="N10" s="36"/>
-      <c r="O10" s="36" t="s">
+      <c r="O10" s="36"/>
+      <c r="P10" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P10" s="39">
+      <c r="Q10" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q10" s="36">
+      <c r="R10" s="36">
         <v>308</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>4</v>
       </c>
@@ -5672,17 +5694,18 @@
         <v>222</v>
       </c>
       <c r="N11" s="36"/>
-      <c r="O11" s="36" t="s">
+      <c r="O11" s="36"/>
+      <c r="P11" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P11" s="39">
+      <c r="Q11" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q11" s="36">
+      <c r="R11" s="36">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>4</v>
       </c>
@@ -5721,17 +5744,18 @@
         <v>223</v>
       </c>
       <c r="N12" s="36"/>
-      <c r="O12" s="36" t="s">
+      <c r="O12" s="36"/>
+      <c r="P12" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P12" s="39">
+      <c r="Q12" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q12" s="36">
+      <c r="R12" s="36">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>4</v>
       </c>
@@ -5771,17 +5795,18 @@
         <v>225</v>
       </c>
       <c r="N13" s="36"/>
-      <c r="O13" s="36" t="s">
+      <c r="O13" s="36"/>
+      <c r="P13" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P13" s="39">
+      <c r="Q13" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q13" s="36">
+      <c r="R13" s="36">
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>4</v>
       </c>
@@ -5821,17 +5846,18 @@
         <v>224</v>
       </c>
       <c r="N14" s="36"/>
-      <c r="O14" s="36" t="s">
+      <c r="O14" s="36"/>
+      <c r="P14" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P14" s="39">
+      <c r="Q14" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q14" s="36">
+      <c r="R14" s="36">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>4</v>
       </c>
@@ -5874,17 +5900,18 @@
         <v>226</v>
       </c>
       <c r="N15" s="36"/>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="36"/>
+      <c r="P15" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P15" s="39">
+      <c r="Q15" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q15" s="36">
+      <c r="R15" s="36">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>4</v>
       </c>
@@ -5927,17 +5954,18 @@
         <v>227</v>
       </c>
       <c r="N16" s="36"/>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="36"/>
+      <c r="P16" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P16" s="39">
+      <c r="Q16" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q16" s="36">
+      <c r="R16" s="36">
         <v>546</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>4</v>
       </c>
@@ -5974,17 +6002,18 @@
         <v>228</v>
       </c>
       <c r="N17" s="36"/>
-      <c r="O17" s="36" t="s">
+      <c r="O17" s="36"/>
+      <c r="P17" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="P17" s="39">
+      <c r="Q17" s="39">
         <v>0.41</v>
       </c>
-      <c r="Q17" s="36">
+      <c r="R17" s="36">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>8</v>
       </c>
@@ -6029,15 +6058,16 @@
       <c r="N18" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="17"/>
+      <c r="P18" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P18" s="28">
+      <c r="Q18" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q18" s="15"/>
-    </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>8</v>
       </c>
@@ -6076,15 +6106,16 @@
       <c r="N19" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="17"/>
+      <c r="P19" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P19" s="28">
+      <c r="Q19" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q19" s="15"/>
-    </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="15"/>
+    </row>
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>8</v>
       </c>
@@ -6129,15 +6160,16 @@
       <c r="N20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O20" s="15" t="s">
+      <c r="O20" s="15"/>
+      <c r="P20" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P20" s="28">
+      <c r="Q20" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q20" s="15"/>
-    </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R20" s="15"/>
+    </row>
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>8</v>
       </c>
@@ -6173,15 +6205,16 @@
       <c r="N21" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="O21" s="22" t="s">
+      <c r="O21" s="22"/>
+      <c r="P21" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="P21" s="29">
+      <c r="Q21" s="29">
         <v>0.34</v>
       </c>
-      <c r="Q21" s="22"/>
-    </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="22"/>
+    </row>
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
@@ -6220,15 +6253,16 @@
       <c r="N22" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="O22" s="15" t="s">
+      <c r="O22" s="15"/>
+      <c r="P22" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P22" s="28">
+      <c r="Q22" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q22" s="15"/>
-    </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>8</v>
       </c>
@@ -6270,15 +6304,16 @@
       <c r="N23" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="O23" s="22" t="s">
+      <c r="O23" s="22"/>
+      <c r="P23" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="P23" s="29">
+      <c r="Q23" s="29">
         <v>0.34</v>
       </c>
-      <c r="Q23" s="22"/>
-    </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="22"/>
+    </row>
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>8</v>
       </c>
@@ -6320,15 +6355,16 @@
       <c r="N24" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="O24" s="22" t="s">
+      <c r="O24" s="22"/>
+      <c r="P24" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="P24" s="29">
+      <c r="Q24" s="29">
         <v>0.34</v>
       </c>
-      <c r="Q24" s="22"/>
-    </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>8</v>
       </c>
@@ -6373,15 +6409,16 @@
       <c r="N25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="15"/>
+      <c r="P25" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P25" s="28">
+      <c r="Q25" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q25" s="15"/>
-    </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>8</v>
       </c>
@@ -6426,15 +6463,16 @@
       <c r="N26" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="15"/>
+      <c r="P26" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P26" s="28">
+      <c r="Q26" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q26" s="15"/>
-    </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="15"/>
+    </row>
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>8</v>
       </c>
@@ -6473,15 +6511,16 @@
       <c r="N27" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="O27" s="15" t="s">
+      <c r="O27" s="15"/>
+      <c r="P27" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P27" s="28">
+      <c r="Q27" s="28">
         <v>0.34</v>
       </c>
-      <c r="Q27" s="15"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="15"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>4</v>
       </c>
@@ -6526,15 +6565,16 @@
       <c r="N28" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="O28" s="15" t="s">
+      <c r="O28" s="15"/>
+      <c r="P28" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P28" s="28">
+      <c r="Q28" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q28" s="15"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="15"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>4</v>
       </c>
@@ -6579,15 +6619,16 @@
       <c r="N29" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="O29" s="15" t="s">
+      <c r="O29" s="15"/>
+      <c r="P29" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P29" s="28">
+      <c r="Q29" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q29" s="15"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="15"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>4</v>
       </c>
@@ -6632,15 +6673,16 @@
       <c r="N30" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="O30" s="15" t="s">
+      <c r="O30" s="15"/>
+      <c r="P30" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P30" s="28">
+      <c r="Q30" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q30" s="15"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="15"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>4</v>
       </c>
@@ -6685,15 +6727,16 @@
       <c r="N31" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="O31" s="15" t="s">
+      <c r="O31" s="15"/>
+      <c r="P31" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="P31" s="28">
+      <c r="Q31" s="28">
         <v>0.41</v>
       </c>
-      <c r="Q31" s="15"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="15"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>4</v>
       </c>
@@ -6726,15 +6769,16 @@
       <c r="N32" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="O32" s="13"/>
+      <c r="P32" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P32" s="30">
+      <c r="Q32" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q32" s="5"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="5"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -6767,15 +6811,16 @@
       <c r="N33" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="O33" s="5" t="s">
+      <c r="O33" s="13"/>
+      <c r="P33" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P33" s="30">
+      <c r="Q33" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q33" s="5"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="5"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
@@ -6808,15 +6853,16 @@
       <c r="N34" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="O34" s="5" t="s">
+      <c r="O34" s="5"/>
+      <c r="P34" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P34" s="30">
+      <c r="Q34" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q34" s="5"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="5"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
@@ -6849,15 +6895,16 @@
       <c r="N35" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="O35" s="5" t="s">
+      <c r="O35" s="13"/>
+      <c r="P35" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P35" s="30">
+      <c r="Q35" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q35" s="5"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="5"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
@@ -6890,15 +6937,16 @@
       <c r="N36" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="O36" s="5" t="s">
+      <c r="O36" s="13"/>
+      <c r="P36" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P36" s="30">
+      <c r="Q36" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q36" s="5"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="5"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -6931,15 +6979,16 @@
       <c r="N37" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="O37" s="5" t="s">
+      <c r="O37" s="13"/>
+      <c r="P37" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P37" s="30">
+      <c r="Q37" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q37" s="5"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="5"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>4</v>
       </c>
@@ -6972,15 +7021,16 @@
       <c r="N38" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="O38" s="5" t="s">
+      <c r="O38" s="13"/>
+      <c r="P38" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P38" s="30">
+      <c r="Q38" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q38" s="5"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="5"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
@@ -7013,15 +7063,16 @@
       <c r="N39" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="O39" s="5"/>
+      <c r="P39" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P39" s="30">
+      <c r="Q39" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q39" s="5"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="5"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
@@ -7054,15 +7105,16 @@
       <c r="N40" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="O40" s="5" t="s">
+      <c r="O40" s="13"/>
+      <c r="P40" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P40" s="30">
+      <c r="Q40" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q40" s="5"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="5"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
@@ -7095,15 +7147,16 @@
       <c r="N41" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="O41" s="5" t="s">
+      <c r="O41" s="13"/>
+      <c r="P41" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P41" s="30">
+      <c r="Q41" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q41" s="5"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="5"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -7136,15 +7189,16 @@
       <c r="N42" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O42" s="13"/>
+      <c r="P42" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="P42" s="30">
+      <c r="Q42" s="30">
         <v>0.41</v>
       </c>
-      <c r="Q42" s="5"/>
-    </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="5"/>
+    </row>
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>8</v>
       </c>
@@ -7177,15 +7231,16 @@
       <c r="N43" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="O43" s="25" t="s">
+      <c r="O43" s="25"/>
+      <c r="P43" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P43" s="31">
+      <c r="Q43" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q43" s="5"/>
-    </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R43" s="5"/>
+    </row>
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>8</v>
       </c>
@@ -7218,15 +7273,16 @@
       <c r="N44" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="O44" s="25" t="s">
+      <c r="O44" s="25"/>
+      <c r="P44" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P44" s="31">
+      <c r="Q44" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q44" s="5"/>
-    </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R44" s="5"/>
+    </row>
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>8</v>
       </c>
@@ -7259,15 +7315,16 @@
       <c r="N45" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="O45" s="25" t="s">
+      <c r="O45" s="25"/>
+      <c r="P45" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P45" s="31">
+      <c r="Q45" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q45" s="5"/>
-    </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R45" s="5"/>
+    </row>
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>8</v>
       </c>
@@ -7300,15 +7357,16 @@
       <c r="N46" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="O46" s="25" t="s">
+      <c r="O46" s="25"/>
+      <c r="P46" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P46" s="31">
+      <c r="Q46" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q46" s="5"/>
-    </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R46" s="5"/>
+    </row>
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>8</v>
       </c>
@@ -7341,15 +7399,16 @@
       <c r="N47" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="O47" s="25" t="s">
+      <c r="O47" s="25"/>
+      <c r="P47" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P47" s="31">
+      <c r="Q47" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q47" s="5"/>
-    </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R47" s="5"/>
+    </row>
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>8</v>
       </c>
@@ -7382,15 +7441,16 @@
       <c r="N48" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="O48" s="25" t="s">
+      <c r="O48" s="25"/>
+      <c r="P48" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P48" s="31">
+      <c r="Q48" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q48" s="5"/>
-    </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R48" s="5"/>
+    </row>
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>8</v>
       </c>
@@ -7423,15 +7483,16 @@
       <c r="N49" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="O49" s="25" t="s">
+      <c r="O49" s="25"/>
+      <c r="P49" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P49" s="31">
+      <c r="Q49" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q49" s="5"/>
-    </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R49" s="5"/>
+    </row>
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>8</v>
       </c>
@@ -7464,15 +7525,16 @@
       <c r="N50" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="O50" s="25" t="s">
+      <c r="O50" s="27"/>
+      <c r="P50" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P50" s="31">
+      <c r="Q50" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q50" s="5"/>
-    </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R50" s="5"/>
+    </row>
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>8</v>
       </c>
@@ -7505,15 +7567,16 @@
       <c r="N51" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="O51" s="25" t="s">
+      <c r="O51" s="25"/>
+      <c r="P51" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P51" s="31">
+      <c r="Q51" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q51" s="5"/>
-    </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R51" s="5"/>
+    </row>
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>8</v>
       </c>
@@ -7546,16 +7609,17 @@
       <c r="N52" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="O52" s="25" t="s">
+      <c r="O52" s="25"/>
+      <c r="P52" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="P52" s="31">
+      <c r="Q52" s="31">
         <v>0.34</v>
       </c>
-      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q52" xr:uid="{EB033180-4452-49A4-8BEB-F48FDF308044}">
+  <autoFilter ref="A1:R52" xr:uid="{EB033180-4452-49A4-8BEB-F48FDF308044}">
     <filterColumn colId="0">
       <filters>
         <filter val="Gerber"/>
@@ -7588,10 +7652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C581B3-4A49-4D7E-AF67-B0CA84DD1A3A}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7601,11 +7665,13 @@
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" customWidth="1"/>
+    <col min="14" max="14" width="100.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -7646,19 +7712,22 @@
         <v>19</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
@@ -7691,19 +7760,22 @@
       <c r="L2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5">
         <v>206.63</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
@@ -7737,18 +7809,19 @@
         <v>121</v>
       </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5">
         <v>224.85999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -7782,18 +7855,19 @@
         <v>122</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5">
         <v>317.63</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
@@ -7825,18 +7899,19 @@
         <v>123</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
         <v>354.87</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
@@ -7870,18 +7945,19 @@
         <v>124</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5">
         <v>357.52</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -7915,18 +7991,19 @@
         <v>125</v>
       </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="5">
+      <c r="P7" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5">
         <v>644.74</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -7960,18 +8037,19 @@
         <v>126</v>
       </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="5">
+      <c r="P8" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="11">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="11">
         <v>52.257166153334992</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
@@ -8005,18 +8083,19 @@
         <v>143</v>
       </c>
       <c r="M9" s="5"/>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="5">
+      <c r="P9" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="11">
+      <c r="Q9" s="5"/>
+      <c r="R9" s="11">
         <v>90.068346141637491</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -8050,18 +8129,19 @@
         <v>144</v>
       </c>
       <c r="M10" s="5"/>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P10" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="11">
+      <c r="Q10" s="5"/>
+      <c r="R10" s="11">
         <v>39.382151105261244</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -8095,18 +8175,19 @@
         <v>129</v>
       </c>
       <c r="M11" s="5"/>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="11">
+      <c r="Q11" s="5"/>
+      <c r="R11" s="11">
         <v>165.65897915102249</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -8140,18 +8221,19 @@
         <v>130</v>
       </c>
       <c r="M12" s="5"/>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="11">
+      <c r="Q12" s="5"/>
+      <c r="R12" s="11">
         <v>117.11139459698248</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -8185,18 +8267,19 @@
         <v>131</v>
       </c>
       <c r="M13" s="5"/>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="11">
+      <c r="Q13" s="5"/>
+      <c r="R13" s="11">
         <v>41.3095536973387</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -8230,18 +8313,19 @@
         <v>248</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="5"/>
+      <c r="O14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="11">
+      <c r="Q14" s="5"/>
+      <c r="R14" s="11">
         <v>41.309324999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -8275,18 +8359,19 @@
         <v>132</v>
       </c>
       <c r="M15" s="5"/>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="11">
+      <c r="Q15" s="5"/>
+      <c r="R15" s="11">
         <v>94.481695102577731</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
@@ -8320,18 +8405,19 @@
         <v>133</v>
       </c>
       <c r="M16" s="5"/>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="5"/>
+      <c r="O16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="11">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="11">
         <v>54.817767294848409</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -8365,18 +8451,19 @@
         <v>134</v>
       </c>
       <c r="M17" s="5"/>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="5"/>
+      <c r="O17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="11">
+      <c r="Q17" s="5"/>
+      <c r="R17" s="11">
         <v>47.024419817793579</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
@@ -8410,18 +8497,19 @@
         <v>135</v>
       </c>
       <c r="M18" s="5"/>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="5"/>
+      <c r="O18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="11">
+      <c r="Q18" s="5"/>
+      <c r="R18" s="11">
         <v>212.23939813904951</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -8455,18 +8543,19 @@
         <v>136</v>
       </c>
       <c r="M19" s="5"/>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="5">
+      <c r="P19" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="11">
+      <c r="Q19" s="5"/>
+      <c r="R19" s="11">
         <v>49.064810425312494</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
@@ -8500,18 +8589,19 @@
         <v>137</v>
       </c>
       <c r="M20" s="5"/>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="5"/>
+      <c r="O20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O20" s="5">
+      <c r="P20" s="5">
         <v>0.42749999999999999</v>
       </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="11">
+      <c r="Q20" s="5"/>
+      <c r="R20" s="11">
         <v>117.11139459698248</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
@@ -8533,12 +8623,13 @@
         <v>246</v>
       </c>
       <c r="M21" s="5"/>
-      <c r="N21" s="14"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -8560,12 +8651,13 @@
         <v>247</v>
       </c>
       <c r="M22" s="5"/>
-      <c r="N22" s="14"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -8587,12 +8679,13 @@
         <v>158</v>
       </c>
       <c r="M23" s="5"/>
-      <c r="N23" s="14"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -8614,12 +8707,13 @@
         <v>157</v>
       </c>
       <c r="M24" s="5"/>
-      <c r="N24" s="14"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -8641,12 +8735,13 @@
         <v>159</v>
       </c>
       <c r="M25" s="5"/>
-      <c r="N25" s="14"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -8668,12 +8763,13 @@
         <v>160</v>
       </c>
       <c r="M26" s="5"/>
-      <c r="N26" s="14"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
@@ -8695,12 +8791,13 @@
         <v>161</v>
       </c>
       <c r="M27" s="5"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
@@ -8722,12 +8819,13 @@
         <v>162</v>
       </c>
       <c r="M28" s="5"/>
-      <c r="N28" s="14"/>
+      <c r="N28" s="5"/>
       <c r="O28" s="14"/>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
@@ -8749,12 +8847,13 @@
         <v>163</v>
       </c>
       <c r="M29" s="5"/>
-      <c r="N29" s="14"/>
+      <c r="N29" s="5"/>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="14"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
@@ -8776,12 +8875,13 @@
         <v>164</v>
       </c>
       <c r="M30" s="5"/>
-      <c r="N30" s="14"/>
+      <c r="N30" s="5"/>
       <c r="O30" s="14"/>
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="14"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -8803,14 +8903,18 @@
         <v>165</v>
       </c>
       <c r="M31" s="5"/>
-      <c r="N31" s="14"/>
+      <c r="N31" s="5"/>
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{6B464FC2-D195-4FF7-BC5B-B0CBC9FFD99F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Lowes pages and autoscraper
</commit_message>
<xml_diff>
--- a/XX_Master_database/Wholesaler_Database.xlsx
+++ b/XX_Master_database/Wholesaler_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/00_Scrapping_git/XX_Master_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1453" documentId="8_{B63EC7D8-7803-4775-989F-2C2416119993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A72EBF33-37F3-4F92-9DF8-703553D88A34}"/>
+  <xr:revisionPtr revIDLastSave="1455" documentId="8_{B63EC7D8-7803-4775-989F-2C2416119993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2628352-0777-442E-9D56-8360547E9846}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{BB750D66-C71B-4412-8809-92E47E37BD8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BB750D66-C71B-4412-8809-92E47E37BD8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitors" sheetId="1" r:id="rId1"/>
@@ -497,9 +497,6 @@
     <t>239 4" MS ROUND LAV</t>
   </si>
   <si>
-    <t xml:space="preserve">348 4" LAV                                                          </t>
-  </si>
-  <si>
     <t>272 4" LAV</t>
   </si>
   <si>
@@ -947,7 +944,10 @@
     <t>ALTO BOWL 130 1.6</t>
   </si>
   <si>
-    <t>COMEMRCIAL BOWL 1319 EL  1.28</t>
+    <t>COMMERCIAL BOWL 1319 EL  1.28</t>
+  </si>
+  <si>
+    <t>348 4" LAV</t>
   </si>
 </sst>
 </file>
@@ -5148,7 +5148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB033180-4452-49A4-8BEB-F48FDF308044}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
@@ -5196,10 +5196,10 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
@@ -5217,7 +5217,7 @@
         <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>20</v>
@@ -5226,7 +5226,7 @@
         <v>3</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="O2" s="12"/>
       <c r="P2" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="25">
         <v>0.41</v>
@@ -5328,11 +5328,11 @@
         <v>101</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q3" s="25">
         <v>0.41</v>
@@ -5383,11 +5383,11 @@
         <v>102</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q4" s="25">
         <v>0.41</v>
@@ -5441,7 +5441,7 @@
       </c>
       <c r="O5" s="14"/>
       <c r="P5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q5" s="25">
         <v>0.34</v>
@@ -5496,7 +5496,7 @@
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q6" s="25">
         <v>0.34</v>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q7" s="25">
         <v>0.34</v>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="O8" s="12"/>
       <c r="P8" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q8" s="25">
         <v>0.34</v>
@@ -5657,11 +5657,11 @@
         <v>111</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q9" s="25">
         <v>0.34</v>
@@ -5684,7 +5684,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>31</v>
@@ -5705,14 +5705,14 @@
         <v>1.6</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N10" s="31"/>
       <c r="O10" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P10" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q10" s="34">
         <v>0.41</v>
@@ -5726,7 +5726,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31">
@@ -5754,14 +5754,14 @@
         <v>1.28</v>
       </c>
       <c r="M11" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N11" s="31"/>
       <c r="O11" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P11" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q11" s="34">
         <v>0.41</v>
@@ -5786,7 +5786,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F12" s="31" t="s">
         <v>31</v>
@@ -5806,14 +5806,14 @@
         <v>1.6</v>
       </c>
       <c r="M12" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N12" s="31"/>
       <c r="O12" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P12" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q12" s="34">
         <v>0.41</v>
@@ -5827,7 +5827,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31">
@@ -5859,14 +5859,14 @@
         <v>1.28</v>
       </c>
       <c r="M13" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N13" s="31"/>
       <c r="O13" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P13" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q13" s="34">
         <v>0.41</v>
@@ -5880,7 +5880,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31">
@@ -5912,14 +5912,14 @@
         <v>1.28</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P14" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q14" s="34">
         <v>0.41</v>
@@ -5944,7 +5944,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>31</v>
@@ -5968,14 +5968,14 @@
         <v>1.6</v>
       </c>
       <c r="M15" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N15" s="31"/>
       <c r="O15" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q15" s="34">
         <v>0.41</v>
@@ -6000,7 +6000,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>33</v>
@@ -6009,7 +6009,7 @@
         <v>46</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I16" s="33">
         <v>12</v>
@@ -6021,17 +6021,17 @@
         <v>53</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M16" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N16" s="31"/>
       <c r="O16" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P16" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q16" s="34">
         <v>0.41</v>
@@ -6056,7 +6056,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>30</v>
@@ -6074,14 +6074,14 @@
         <v>1.6</v>
       </c>
       <c r="M17" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N17" s="31"/>
       <c r="O17" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P17" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q17" s="34">
         <v>0.41</v>
@@ -6130,14 +6130,14 @@
         <v>1.6</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N18" s="14" t="s">
         <v>100</v>
       </c>
       <c r="O18" s="14"/>
       <c r="P18" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q18" s="25">
         <v>0.34</v>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="O19" s="14"/>
       <c r="P19" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q19" s="25">
         <v>0.34</v>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="C20" s="12" t="str">
         <f>VLOOKUP(B20,Mansfield!$D$1:$L$20,9,0)</f>
-        <v>COMEMRCIAL BOWL 1319 EL  1.28</v>
+        <v>COMMERCIAL BOWL 1319 EL  1.28</v>
       </c>
       <c r="D20" s="12">
         <f t="shared" si="0"/>
@@ -6229,7 +6229,7 @@
         <v>53</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>115</v>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q20" s="25">
         <v>0.34</v>
@@ -6251,7 +6251,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="O21" s="19"/>
       <c r="P21" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q21" s="26">
         <v>0.34</v>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q22" s="25">
         <v>0.34</v>
@@ -6344,7 +6344,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="O23" s="19"/>
       <c r="P23" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q23" s="26">
         <v>0.34</v>
@@ -6395,7 +6395,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="O24" s="19"/>
       <c r="P24" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q24" s="26">
         <v>0.34</v>
@@ -6488,7 +6488,7 @@
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q25" s="25">
         <v>0.34</v>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="O26" s="12"/>
       <c r="P26" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q26" s="25">
         <v>0.34</v>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q27" s="25">
         <v>0.34</v>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="C28" s="12" t="str">
         <f>VLOOKUP(B28,Mansfield!$D$1:$L$20,9,0)</f>
-        <v>COMEMRCIAL BOWL 1319 EL  1.28</v>
+        <v>COMMERCIAL BOWL 1319 EL  1.28</v>
       </c>
       <c r="D28" s="12">
         <f t="shared" si="0"/>
@@ -6644,7 +6644,7 @@
       </c>
       <c r="O28" s="12"/>
       <c r="P28" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q28" s="25">
         <v>0.41</v>
@@ -6698,7 +6698,7 @@
       </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q29" s="25">
         <v>0.41</v>
@@ -6752,7 +6752,7 @@
       </c>
       <c r="O30" s="12"/>
       <c r="P30" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q30" s="25">
         <v>0.41</v>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="O31" s="12"/>
       <c r="P31" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q31" s="25">
         <v>0.41</v>
@@ -6818,7 +6818,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="9" t="str">
         <f>VLOOKUP(B32,Mansfield!$D$1:$L$50,9,0)</f>
@@ -6841,14 +6841,14 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O32" s="10"/>
       <c r="P32" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q32" s="27">
         <v>0.41</v>
@@ -6860,7 +6860,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" s="9" t="str">
         <f>VLOOKUP(B33,Mansfield!$D$1:$L$50,9,0)</f>
@@ -6883,14 +6883,14 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O33" s="10"/>
       <c r="P33" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q33" s="27">
         <v>0.41</v>
@@ -6902,7 +6902,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="9" t="str">
         <f>VLOOKUP(B34,Mansfield!$D$1:$L$50,9,0)</f>
@@ -6925,14 +6925,14 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q34" s="27">
         <v>0.41</v>
@@ -6944,7 +6944,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" s="9" t="str">
         <f>VLOOKUP(B35,Mansfield!$D$1:$L$50,9,0)</f>
@@ -6967,14 +6967,14 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q35" s="27">
         <v>0.41</v>
@@ -6986,7 +6986,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" s="9" t="str">
         <f>VLOOKUP(B36,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7009,14 +7009,14 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O36" s="10"/>
       <c r="P36" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q36" s="27">
         <v>0.41</v>
@@ -7028,7 +7028,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="9" t="str">
         <f>VLOOKUP(B37,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7051,14 +7051,14 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N37" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O37" s="10"/>
       <c r="P37" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q37" s="27">
         <v>0.41</v>
@@ -7070,11 +7070,11 @@
         <v>4</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="9" t="str">
         <f>VLOOKUP(B38,Mansfield!$D$1:$L$50,9,0)</f>
-        <v xml:space="preserve">348 4" LAV                                                          </v>
+        <v>348 4" LAV</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="1"/>
@@ -7093,14 +7093,14 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O38" s="10"/>
       <c r="P38" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q38" s="27">
         <v>0.41</v>
@@ -7112,7 +7112,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" s="9" t="str">
         <f>VLOOKUP(B39,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7135,14 +7135,14 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q39" s="27">
         <v>0.41</v>
@@ -7154,7 +7154,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="9" t="str">
         <f>VLOOKUP(B40,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7177,14 +7177,14 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N40" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O40" s="10"/>
       <c r="P40" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q40" s="27">
         <v>0.41</v>
@@ -7196,7 +7196,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C41" s="9" t="str">
         <f>VLOOKUP(B41,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7219,14 +7219,14 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O41" s="10"/>
       <c r="P41" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q41" s="27">
         <v>0.41</v>
@@ -7238,7 +7238,7 @@
         <v>4</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C42" s="9" t="str">
         <f>VLOOKUP(B42,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7261,14 +7261,14 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O42" s="10"/>
       <c r="P42" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q42" s="27">
         <v>0.41</v>
@@ -7280,7 +7280,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C43" s="22" t="str">
         <f>VLOOKUP(B43,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7291,7 +7291,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>138</v>
@@ -7303,14 +7303,14 @@
       <c r="K43" s="22"/>
       <c r="L43" s="22"/>
       <c r="M43" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N43" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O43" s="22"/>
       <c r="P43" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q43" s="28">
         <v>0.34</v>
@@ -7322,7 +7322,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C44" s="22" t="str">
         <f>VLOOKUP(B44,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7333,7 +7333,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F44" s="22" t="s">
         <v>138</v>
@@ -7345,14 +7345,14 @@
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N44" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O44" s="22"/>
       <c r="P44" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q44" s="28">
         <v>0.34</v>
@@ -7364,7 +7364,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C45" s="22" t="str">
         <f>VLOOKUP(B45,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7375,7 +7375,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F45" s="22" t="s">
         <v>138</v>
@@ -7387,14 +7387,14 @@
       <c r="K45" s="22"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N45" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O45" s="22"/>
       <c r="P45" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q45" s="28">
         <v>0.34</v>
@@ -7406,7 +7406,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C46" s="22" t="str">
         <f>VLOOKUP(B46,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7417,7 +7417,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F46" s="22" t="s">
         <v>138</v>
@@ -7429,14 +7429,14 @@
       <c r="K46" s="22"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N46" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O46" s="22"/>
       <c r="P46" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q46" s="28">
         <v>0.34</v>
@@ -7448,7 +7448,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C47" s="22" t="str">
         <f>VLOOKUP(B47,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7459,7 +7459,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F47" s="22" t="s">
         <v>138</v>
@@ -7471,14 +7471,14 @@
       <c r="K47" s="22"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N47" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O47" s="22"/>
       <c r="P47" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q47" s="28">
         <v>0.34</v>
@@ -7490,18 +7490,18 @@
         <v>8</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C48" s="22" t="str">
         <f>VLOOKUP(B48,Mansfield!$D$1:$L$50,9,0)</f>
-        <v xml:space="preserve">348 4" LAV                                                          </v>
+        <v>348 4" LAV</v>
       </c>
       <c r="D48" s="22">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>138</v>
@@ -7513,14 +7513,14 @@
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N48" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O48" s="22"/>
       <c r="P48" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q48" s="28">
         <v>0.34</v>
@@ -7532,7 +7532,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C49" s="22" t="str">
         <f>VLOOKUP(B49,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7543,7 +7543,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>138</v>
@@ -7555,14 +7555,14 @@
       <c r="K49" s="22"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N49" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O49" s="22"/>
       <c r="P49" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q49" s="28">
         <v>0.34</v>
@@ -7574,7 +7574,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" s="22" t="str">
         <f>VLOOKUP(B50,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7585,7 +7585,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>138</v>
@@ -7597,14 +7597,14 @@
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N50" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O50" s="24"/>
       <c r="P50" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q50" s="28">
         <v>0.34</v>
@@ -7616,7 +7616,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C51" s="22" t="str">
         <f>VLOOKUP(B51,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7627,7 +7627,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>138</v>
@@ -7639,14 +7639,14 @@
       <c r="K51" s="22"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N51" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O51" s="22"/>
       <c r="P51" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q51" s="28">
         <v>0.34</v>
@@ -7658,7 +7658,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C52" s="22" t="str">
         <f>VLOOKUP(B52,Mansfield!$D$1:$L$50,9,0)</f>
@@ -7669,7 +7669,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>138</v>
@@ -7681,14 +7681,14 @@
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N52" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O52" s="22"/>
       <c r="P52" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q52" s="28">
         <v>0.34</v>
@@ -7730,8 +7730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C581B3-4A49-4D7E-AF67-B0CA84DD1A3A}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7767,10 +7767,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>15</v>
@@ -7788,7 +7788,7 @@
         <v>19</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>20</v>
@@ -7838,10 +7838,10 @@
       </c>
       <c r="M2" s="10"/>
       <c r="N2" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P2" s="3">
         <v>0.42749999999999999</v>
@@ -7886,10 +7886,10 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P3" s="3">
         <v>0.42749999999999999</v>
@@ -7934,10 +7934,10 @@
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P4" s="3">
         <v>0.42749999999999999</v>
@@ -7980,10 +7980,10 @@
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P5" s="3">
         <v>0.42749999999999999</v>
@@ -8028,10 +8028,10 @@
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P6" s="3">
         <v>0.42749999999999999</v>
@@ -8076,10 +8076,10 @@
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P7" s="3">
         <v>0.42749999999999999</v>
@@ -8120,12 +8120,12 @@
         <v>1.28</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P8" s="3">
         <v>0.42749999999999999</v>
@@ -8171,7 +8171,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P9" s="3">
         <v>0.42749999999999999</v>
@@ -8217,7 +8217,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P10" s="3">
         <v>0.42749999999999999</v>
@@ -8258,14 +8258,14 @@
         <v>50</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P11" s="3">
         <v>0.42749999999999999</v>
@@ -8306,14 +8306,14 @@
         <v>50</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P12" s="3">
         <v>0.42749999999999999</v>
@@ -8354,14 +8354,14 @@
         <v>50</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P13" s="3">
         <v>0.42749999999999999</v>
@@ -8402,14 +8402,14 @@
         <v>50</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P14" s="3">
         <v>0.42749999999999999</v>
@@ -8450,14 +8450,14 @@
         <v>1.6</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P15" s="3">
         <v>0.42749999999999999</v>
@@ -8502,10 +8502,10 @@
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P16" s="3">
         <v>0.42749999999999999</v>
@@ -8546,14 +8546,14 @@
         <v>1.6</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P17" s="3">
         <v>0.42749999999999999</v>
@@ -8594,14 +8594,14 @@
         <v>1.6</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P18" s="3">
         <v>0.42749999999999999</v>
@@ -8646,10 +8646,10 @@
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P19" s="3">
         <v>0.42749999999999999</v>
@@ -8694,10 +8694,10 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P20" s="3">
         <v>0.42749999999999999</v>
@@ -8714,7 +8714,7 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>138</v>
@@ -8726,14 +8726,14 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P21" s="3">
         <v>0.42749999999999999</v>
@@ -8750,7 +8750,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>138</v>
@@ -8762,14 +8762,14 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P22" s="3">
         <v>0.42749999999999999</v>
@@ -8786,7 +8786,7 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>138</v>
@@ -8798,14 +8798,14 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P23" s="3">
         <v>0.42749999999999999</v>
@@ -8822,7 +8822,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>138</v>
@@ -8838,10 +8838,10 @@
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P24" s="3">
         <v>0.42749999999999999</v>
@@ -8858,7 +8858,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>138</v>
@@ -8870,14 +8870,14 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P25" s="3">
         <v>0.42749999999999999</v>
@@ -8894,7 +8894,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>138</v>
@@ -8910,10 +8910,10 @@
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P26" s="3">
         <v>0.42749999999999999</v>
@@ -8930,7 +8930,7 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>138</v>
@@ -8942,14 +8942,14 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
-        <v>151</v>
+        <v>301</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P27" s="3">
         <v>0.42749999999999999</v>
@@ -8966,7 +8966,7 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>138</v>
@@ -8978,14 +8978,14 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P28" s="3">
         <v>0.42749999999999999</v>
@@ -9002,7 +9002,7 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>138</v>
@@ -9014,14 +9014,14 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P29" s="3">
         <v>0.42749999999999999</v>
@@ -9038,7 +9038,7 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>138</v>
@@ -9050,14 +9050,14 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P30" s="3">
         <v>0.42749999999999999</v>
@@ -9074,7 +9074,7 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>138</v>
@@ -9086,14 +9086,14 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P31" s="3">
         <v>0.42749999999999999</v>
@@ -9137,22 +9137,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" t="s">
         <v>221</v>
       </c>
-      <c r="B1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" t="s">
-        <v>223</v>
-      </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -9169,7 +9169,7 @@
         <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E2">
         <v>110</v>
@@ -9193,7 +9193,7 @@
         <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E3">
         <v>96.63</v>
@@ -9217,7 +9217,7 @@
         <v>135</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E4">
         <v>128.22999999999999</v>
@@ -9241,7 +9241,7 @@
         <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5">
         <v>0.42749999999999999</v>
@@ -9262,7 +9262,7 @@
         <v>137</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F6">
         <v>0.42749999999999999</v>
@@ -9283,7 +9283,7 @@
         <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7">
         <v>0.42749999999999999</v>
@@ -9304,7 +9304,7 @@
         <v>3151</v>
       </c>
       <c r="D8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F8">
         <v>0.42749999999999999</v>
@@ -9325,7 +9325,7 @@
         <v>3486</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F9">
         <v>0.42749999999999999</v>
@@ -9346,7 +9346,7 @@
         <v>384</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F10">
         <v>0.42749999999999999</v>
@@ -9364,7 +9364,7 @@
         <v>386</v>
       </c>
       <c r="D11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F11">
         <v>0.42749999999999999</v>
@@ -9385,7 +9385,7 @@
         <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F12">
         <v>0.42749999999999999</v>
@@ -9403,7 +9403,7 @@
         <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F13">
         <v>0.42749999999999999</v>

</xml_diff>